<commit_message>
add w11 - redis
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="127">
   <si>
     <t>Alarico Mercado Vázquez</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>ricardo</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Api</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +478,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -520,7 +538,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -529,6 +547,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2042,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2054,99 +2074,105 @@
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" customWidth="1"/>
-    <col min="11" max="11" width="4.1640625" customWidth="1"/>
-    <col min="12" max="12" width="1.5" customWidth="1"/>
-    <col min="13" max="13" width="3.83203125" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" customWidth="1"/>
-    <col min="15" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="3.83203125" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" customWidth="1"/>
-    <col min="19" max="19" width="7" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.1640625" customWidth="1"/>
-    <col min="22" max="22" width="4" customWidth="1"/>
-    <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="5" customWidth="1"/>
-    <col min="25" max="25" width="3.83203125" customWidth="1"/>
-    <col min="26" max="26" width="1.6640625" customWidth="1"/>
-    <col min="27" max="27" width="3.6640625" customWidth="1"/>
-    <col min="28" max="28" width="10.83203125" style="4"/>
+    <col min="6" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="2.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" customWidth="1"/>
+    <col min="13" max="13" width="1.5" customWidth="1"/>
+    <col min="14" max="14" width="3.83203125" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" customWidth="1"/>
+    <col min="16" max="17" width="6" customWidth="1"/>
+    <col min="18" max="18" width="3.83203125" customWidth="1"/>
+    <col min="19" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="20" width="7" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" customWidth="1"/>
+    <col min="23" max="23" width="4" customWidth="1"/>
+    <col min="24" max="24" width="10" customWidth="1"/>
+    <col min="25" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="3.83203125" customWidth="1"/>
+    <col min="27" max="27" width="1.6640625" customWidth="1"/>
+    <col min="28" max="28" width="3.6640625" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>78</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>105</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>93</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>94</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>95</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>97</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>96</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>98</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>99</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>106</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2165,18 +2191,19 @@
       <c r="F2">
         <v>8080</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <f>F2+30</f>
+        <v>8110</v>
+      </c>
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
         <v>1</v>
       </c>
@@ -2190,19 +2217,19 @@
         <v>1</v>
       </c>
       <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
         <v>20</v>
       </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
       <c r="Q2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R2">
         <v>5</v>
       </c>
       <c r="S2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T2">
         <v>10</v>
@@ -2214,27 +2241,30 @@
         <v>10</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X2">
         <v>5</v>
       </c>
       <c r="Y2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Z2">
         <v>10</v>
       </c>
       <c r="AA2">
-        <f>SUM(P2:Z2)*0.8</f>
+        <v>10</v>
+      </c>
+      <c r="AB2">
+        <f>SUM(Q2:AA2)*0.8</f>
         <v>72</v>
       </c>
-      <c r="AB2" s="4">
-        <f>AA2+O2</f>
+      <c r="AC2" s="4">
+        <f>AB2+P2</f>
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2254,18 +2284,19 @@
         <f>F2+1</f>
         <v>8081</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3">
+        <f>G2+1</f>
+        <v>8111</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
         <v>1</v>
       </c>
@@ -2276,22 +2307,22 @@
         <v>1</v>
       </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>16</v>
       </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
       <c r="Q3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R3">
         <v>5</v>
       </c>
       <c r="S3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T3">
         <v>10</v>
@@ -2315,15 +2346,18 @@
         <v>10</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA23" si="0">SUM(P3:Z3)*0.8</f>
+        <v>10</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB23" si="0">SUM(Q3:AA3)*0.8</f>
         <v>80</v>
       </c>
-      <c r="AB3" s="4">
-        <f t="shared" ref="AB3:AB23" si="1">AA3+O3</f>
+      <c r="AC3" s="4">
+        <f t="shared" ref="AC3:AC23" si="1">AB3+P3</f>
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:29">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2340,15 +2374,16 @@
         <v>51</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F23" si="2">F3+1</f>
+        <f t="shared" ref="F4:G23" si="2">F3+1</f>
         <v>8082</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>8112</v>
+      </c>
+      <c r="H4" t="s">
         <v>114</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
       <c r="K4">
         <v>1</v>
       </c>
@@ -2356,25 +2391,25 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>12</v>
       </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
       <c r="Q4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R4">
         <v>5</v>
       </c>
       <c r="S4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T4">
         <v>10</v>
@@ -2398,15 +2433,18 @@
         <v>10</v>
       </c>
       <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AC4" s="4">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:29">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2426,18 +2464,19 @@
         <f t="shared" si="2"/>
         <v>8083</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>8113</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
       <c r="K5">
         <v>1</v>
       </c>
@@ -2451,21 +2490,21 @@
         <v>1</v>
       </c>
       <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <v>20</v>
       </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
       <c r="Q5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R5">
         <v>5</v>
       </c>
-      <c r="S5" s="6">
-        <v>10</v>
-      </c>
-      <c r="T5">
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5" s="6">
         <v>10</v>
       </c>
       <c r="U5">
@@ -2474,10 +2513,10 @@
       <c r="V5">
         <v>10</v>
       </c>
-      <c r="W5" s="6">
-        <v>10</v>
-      </c>
-      <c r="X5">
+      <c r="W5">
+        <v>10</v>
+      </c>
+      <c r="X5" s="6">
         <v>10</v>
       </c>
       <c r="Y5">
@@ -2487,15 +2526,18 @@
         <v>10</v>
       </c>
       <c r="AA5">
+        <v>10</v>
+      </c>
+      <c r="AB5">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AC5" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:29">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2515,18 +2557,19 @@
         <f t="shared" si="2"/>
         <v>8084</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>8114</v>
+      </c>
+      <c r="H6" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
         <v>1</v>
       </c>
@@ -2540,19 +2583,19 @@
         <v>1</v>
       </c>
       <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <v>20</v>
       </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
       <c r="Q6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R6">
         <v>5</v>
       </c>
       <c r="S6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T6">
         <v>10</v>
@@ -2576,15 +2619,18 @@
         <v>10</v>
       </c>
       <c r="AA6">
+        <v>10</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AC6" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:29">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2604,12 +2650,13 @@
         <f t="shared" si="2"/>
         <v>8085</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>8115</v>
+      </c>
+      <c r="H7" t="s">
         <v>118</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7">
         <v>1</v>
       </c>
@@ -2623,21 +2670,21 @@
         <v>1</v>
       </c>
       <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
         <v>20</v>
       </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
       <c r="Q7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R7">
         <v>5</v>
       </c>
-      <c r="S7" s="6">
-        <v>10</v>
-      </c>
-      <c r="T7">
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7" s="6">
         <v>10</v>
       </c>
       <c r="U7">
@@ -2646,10 +2693,10 @@
       <c r="V7">
         <v>10</v>
       </c>
-      <c r="W7" s="6">
-        <v>10</v>
-      </c>
-      <c r="X7">
+      <c r="W7">
+        <v>10</v>
+      </c>
+      <c r="X7" s="6">
         <v>10</v>
       </c>
       <c r="Y7">
@@ -2659,15 +2706,18 @@
         <v>10</v>
       </c>
       <c r="AA7">
+        <v>10</v>
+      </c>
+      <c r="AB7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AC7" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:29">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2687,14 +2737,15 @@
         <f t="shared" si="2"/>
         <v>8086</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>8116</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8">
-        <v>1</v>
-      </c>
+      <c r="J8" s="3"/>
       <c r="K8">
         <v>1</v>
       </c>
@@ -2708,19 +2759,19 @@
         <v>1</v>
       </c>
       <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
         <v>20</v>
       </c>
-      <c r="P8">
-        <v>10</v>
-      </c>
       <c r="Q8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R8">
         <v>5</v>
       </c>
       <c r="S8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T8">
         <v>10</v>
@@ -2744,15 +2795,18 @@
         <v>10</v>
       </c>
       <c r="AA8">
+        <v>10</v>
+      </c>
+      <c r="AB8">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="AC8" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:29">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2772,12 +2826,13 @@
         <f t="shared" si="2"/>
         <v>8087</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>8117</v>
+      </c>
+      <c r="H9" t="s">
         <v>73</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
       <c r="K9">
         <v>1</v>
       </c>
@@ -2791,19 +2846,19 @@
         <v>1</v>
       </c>
       <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
         <v>20</v>
       </c>
-      <c r="P9">
-        <v>10</v>
-      </c>
       <c r="Q9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R9">
         <v>5</v>
       </c>
       <c r="S9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T9">
         <v>10</v>
@@ -2827,15 +2882,18 @@
         <v>10</v>
       </c>
       <c r="AA9">
+        <v>10</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AC9" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:29">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2855,12 +2913,13 @@
         <f t="shared" si="2"/>
         <v>8088</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>8118</v>
+      </c>
+      <c r="H10" t="s">
         <v>74</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
       <c r="K10">
         <v>1</v>
       </c>
@@ -2874,19 +2933,19 @@
         <v>1</v>
       </c>
       <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
         <v>20</v>
       </c>
-      <c r="P10">
-        <v>10</v>
-      </c>
       <c r="Q10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R10">
         <v>5</v>
       </c>
       <c r="S10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T10">
         <v>10</v>
@@ -2910,15 +2969,18 @@
         <v>10</v>
       </c>
       <c r="AA10">
+        <v>10</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AC10" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:29">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2938,12 +3000,13 @@
         <f t="shared" si="2"/>
         <v>8089</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>8119</v>
+      </c>
+      <c r="H11" t="s">
         <v>86</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
       <c r="K11">
         <v>1</v>
       </c>
@@ -2954,22 +3017,22 @@
         <v>1</v>
       </c>
       <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
         <v>0</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>20</v>
       </c>
-      <c r="P11">
-        <v>10</v>
-      </c>
       <c r="Q11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R11">
         <v>5</v>
       </c>
       <c r="S11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T11">
         <v>10</v>
@@ -2993,15 +3056,18 @@
         <v>10</v>
       </c>
       <c r="AA11">
+        <v>10</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="AC11" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:29">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3021,12 +3087,13 @@
         <f t="shared" si="2"/>
         <v>8090</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>8120</v>
+      </c>
+      <c r="H12" t="s">
         <v>85</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
       <c r="K12">
         <v>1</v>
       </c>
@@ -3040,19 +3107,19 @@
         <v>1</v>
       </c>
       <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
         <v>20</v>
       </c>
-      <c r="P12">
-        <v>10</v>
-      </c>
       <c r="Q12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R12">
         <v>5</v>
       </c>
       <c r="S12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T12">
         <v>10</v>
@@ -3064,27 +3131,30 @@
         <v>10</v>
       </c>
       <c r="W12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X12">
         <v>5</v>
       </c>
       <c r="Y12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Z12">
         <v>10</v>
       </c>
       <c r="AA12">
-        <f>SUM(P12:Z12)*0.8</f>
+        <v>10</v>
+      </c>
+      <c r="AB12">
+        <f>SUM(Q12:AA12)*0.8</f>
         <v>72</v>
       </c>
-      <c r="AB12" s="4">
+      <c r="AC12" s="4">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:29">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3104,12 +3174,13 @@
         <f t="shared" si="2"/>
         <v>8091</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>8121</v>
+      </c>
+      <c r="H13" t="s">
         <v>87</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
       <c r="K13">
         <v>1</v>
       </c>
@@ -3123,19 +3194,19 @@
         <v>1</v>
       </c>
       <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
         <v>20</v>
       </c>
-      <c r="P13">
-        <v>10</v>
-      </c>
       <c r="Q13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R13">
         <v>5</v>
       </c>
       <c r="S13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T13">
         <v>10</v>
@@ -3147,27 +3218,30 @@
         <v>10</v>
       </c>
       <c r="W13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X13">
         <v>5</v>
       </c>
       <c r="Y13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Z13">
         <v>10</v>
       </c>
       <c r="AA13">
-        <f>SUM(P13:Z13)*0.8</f>
+        <v>10</v>
+      </c>
+      <c r="AB13">
+        <f>SUM(Q13:AA13)*0.8</f>
         <v>72</v>
       </c>
-      <c r="AB13" s="4">
+      <c r="AC13" s="4">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:29">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3187,33 +3261,34 @@
         <f t="shared" si="2"/>
         <v>8092</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>8122</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14">
-        <v>0</v>
-      </c>
+      <c r="J14" s="1"/>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="P14" s="5">
-        <v>10</v>
+      <c r="M14">
+        <v>0</v>
       </c>
       <c r="Q14" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R14" s="5">
         <v>5</v>
       </c>
-      <c r="S14" s="7">
-        <v>10</v>
-      </c>
-      <c r="T14" s="5">
+      <c r="S14" s="5">
+        <v>5</v>
+      </c>
+      <c r="T14" s="7">
         <v>10</v>
       </c>
       <c r="U14" s="5">
@@ -3222,10 +3297,10 @@
       <c r="V14" s="5">
         <v>10</v>
       </c>
-      <c r="W14" s="7">
-        <v>10</v>
-      </c>
-      <c r="X14" s="5">
+      <c r="W14" s="5">
+        <v>10</v>
+      </c>
+      <c r="X14" s="7">
         <v>10</v>
       </c>
       <c r="Y14" s="5">
@@ -3234,16 +3309,19 @@
       <c r="Z14" s="5">
         <v>10</v>
       </c>
-      <c r="AA14">
+      <c r="AA14" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB14">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB14" s="4">
+      <c r="AC14" s="4">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:29">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3263,12 +3341,13 @@
         <f t="shared" si="2"/>
         <v>8093</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>8123</v>
+      </c>
+      <c r="H15" t="s">
         <v>77</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
       <c r="K15">
         <v>1</v>
       </c>
@@ -3282,21 +3361,21 @@
         <v>1</v>
       </c>
       <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <v>20</v>
       </c>
-      <c r="P15" s="5">
-        <v>10</v>
-      </c>
       <c r="Q15" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
-      <c r="S15" s="7">
-        <v>10</v>
-      </c>
-      <c r="T15" s="5">
+      <c r="S15" s="5">
+        <v>5</v>
+      </c>
+      <c r="T15" s="7">
         <v>10</v>
       </c>
       <c r="U15" s="5">
@@ -3305,10 +3384,10 @@
       <c r="V15" s="5">
         <v>10</v>
       </c>
-      <c r="W15" s="7">
-        <v>10</v>
-      </c>
-      <c r="X15" s="5">
+      <c r="W15" s="5">
+        <v>10</v>
+      </c>
+      <c r="X15" s="7">
         <v>10</v>
       </c>
       <c r="Y15" s="5">
@@ -3317,16 +3396,19 @@
       <c r="Z15" s="5">
         <v>10</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB15">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="AC15" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:29">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3346,12 +3428,13 @@
         <f t="shared" si="2"/>
         <v>8094</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>8124</v>
+      </c>
+      <c r="H16" t="s">
         <v>72</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
       <c r="K16">
         <v>1</v>
       </c>
@@ -3365,19 +3448,19 @@
         <v>1</v>
       </c>
       <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
         <v>20</v>
       </c>
-      <c r="P16" s="5">
-        <v>10</v>
-      </c>
       <c r="Q16" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R16" s="5">
         <v>5</v>
       </c>
       <c r="S16" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T16" s="5">
         <v>10</v>
@@ -3400,16 +3483,19 @@
       <c r="Z16" s="5">
         <v>10</v>
       </c>
-      <c r="AA16">
+      <c r="AA16" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB16">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB16" s="4">
+      <c r="AC16" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:29">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3429,14 +3515,15 @@
         <f t="shared" si="2"/>
         <v>8095</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>8125</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17">
-        <v>1</v>
-      </c>
+      <c r="J17" s="3"/>
       <c r="K17">
         <v>1</v>
       </c>
@@ -3450,19 +3537,19 @@
         <v>1</v>
       </c>
       <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
         <v>20</v>
       </c>
-      <c r="P17" s="5">
-        <v>10</v>
-      </c>
       <c r="Q17" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R17" s="5">
         <v>5</v>
       </c>
       <c r="S17" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T17" s="5">
         <v>10</v>
@@ -3485,16 +3572,19 @@
       <c r="Z17" s="5">
         <v>10</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB17">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB17" s="4">
+      <c r="AC17" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:29">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3514,12 +3604,13 @@
         <f t="shared" si="2"/>
         <v>8096</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>8126</v>
+      </c>
+      <c r="H18" t="s">
         <v>83</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
       <c r="K18">
         <v>1</v>
       </c>
@@ -3533,19 +3624,19 @@
         <v>1</v>
       </c>
       <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
         <v>20</v>
       </c>
-      <c r="P18" s="5">
-        <v>10</v>
-      </c>
       <c r="Q18" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R18" s="5">
         <v>5</v>
       </c>
       <c r="S18" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T18" s="5">
         <v>10</v>
@@ -3568,16 +3659,19 @@
       <c r="Z18" s="5">
         <v>10</v>
       </c>
-      <c r="AA18">
+      <c r="AA18" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB18" s="4">
+      <c r="AC18" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:29">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3597,12 +3691,13 @@
         <f t="shared" si="2"/>
         <v>8097</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>8127</v>
+      </c>
+      <c r="H19" t="s">
         <v>84</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
       <c r="K19">
         <v>1</v>
       </c>
@@ -3616,21 +3711,21 @@
         <v>1</v>
       </c>
       <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
         <v>20</v>
       </c>
-      <c r="P19" s="5">
-        <v>10</v>
-      </c>
       <c r="Q19" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R19" s="5">
         <v>5</v>
       </c>
-      <c r="S19" s="7">
-        <v>10</v>
-      </c>
-      <c r="T19" s="5">
+      <c r="S19" s="5">
+        <v>5</v>
+      </c>
+      <c r="T19" s="7">
         <v>10</v>
       </c>
       <c r="U19" s="5">
@@ -3639,10 +3734,10 @@
       <c r="V19" s="5">
         <v>10</v>
       </c>
-      <c r="W19" s="7">
-        <v>10</v>
-      </c>
-      <c r="X19" s="5">
+      <c r="W19" s="5">
+        <v>10</v>
+      </c>
+      <c r="X19" s="7">
         <v>10</v>
       </c>
       <c r="Y19" s="5">
@@ -3651,16 +3746,19 @@
       <c r="Z19" s="5">
         <v>10</v>
       </c>
-      <c r="AA19">
+      <c r="AA19" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB19">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB19" s="4">
+      <c r="AC19" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:29">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3680,12 +3778,13 @@
         <f t="shared" si="2"/>
         <v>8098</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>8128</v>
+      </c>
+      <c r="H20" t="s">
         <v>76</v>
       </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
       <c r="K20">
         <v>1</v>
       </c>
@@ -3699,21 +3798,21 @@
         <v>1</v>
       </c>
       <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
         <v>20</v>
       </c>
-      <c r="P20" s="5">
-        <v>10</v>
-      </c>
       <c r="Q20" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R20" s="5">
         <v>5</v>
       </c>
-      <c r="S20" s="7">
-        <v>10</v>
-      </c>
-      <c r="T20" s="5">
+      <c r="S20" s="5">
+        <v>5</v>
+      </c>
+      <c r="T20" s="7">
         <v>10</v>
       </c>
       <c r="U20" s="5">
@@ -3722,10 +3821,10 @@
       <c r="V20" s="5">
         <v>10</v>
       </c>
-      <c r="W20" s="7">
-        <v>10</v>
-      </c>
-      <c r="X20" s="5">
+      <c r="W20" s="5">
+        <v>10</v>
+      </c>
+      <c r="X20" s="7">
         <v>10</v>
       </c>
       <c r="Y20" s="5">
@@ -3734,16 +3833,19 @@
       <c r="Z20" s="5">
         <v>10</v>
       </c>
-      <c r="AA20">
+      <c r="AA20" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB20">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB20" s="4">
+      <c r="AC20" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:29">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3763,12 +3865,13 @@
         <f t="shared" si="2"/>
         <v>8099</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>8129</v>
+      </c>
+      <c r="H21" t="s">
         <v>79</v>
       </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
       <c r="K21">
         <v>1</v>
       </c>
@@ -3782,21 +3885,21 @@
         <v>1</v>
       </c>
       <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
         <v>20</v>
       </c>
-      <c r="P21" s="5">
-        <v>10</v>
-      </c>
       <c r="Q21" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R21" s="5">
         <v>5</v>
       </c>
-      <c r="S21" s="7">
-        <v>10</v>
-      </c>
-      <c r="T21" s="5">
+      <c r="S21" s="5">
+        <v>5</v>
+      </c>
+      <c r="T21" s="7">
         <v>10</v>
       </c>
       <c r="U21" s="5">
@@ -3805,10 +3908,10 @@
       <c r="V21" s="5">
         <v>10</v>
       </c>
-      <c r="W21" s="7">
-        <v>10</v>
-      </c>
-      <c r="X21" s="5">
+      <c r="W21" s="5">
+        <v>10</v>
+      </c>
+      <c r="X21" s="7">
         <v>10</v>
       </c>
       <c r="Y21" s="5">
@@ -3817,16 +3920,19 @@
       <c r="Z21" s="5">
         <v>10</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB21" s="4">
+      <c r="AC21" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:29">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3846,12 +3952,13 @@
         <f t="shared" si="2"/>
         <v>8100</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>8130</v>
+      </c>
+      <c r="H22" t="s">
         <v>81</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
       <c r="K22">
         <v>1</v>
       </c>
@@ -3864,20 +3971,20 @@
       <c r="N22">
         <v>1</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="5">
         <v>20</v>
       </c>
-      <c r="P22" s="5">
-        <v>10</v>
-      </c>
       <c r="Q22" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R22" s="5">
         <v>5</v>
       </c>
       <c r="S22" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T22" s="5">
         <v>10</v>
@@ -3889,27 +3996,30 @@
         <v>10</v>
       </c>
       <c r="W22" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X22" s="5">
         <v>5</v>
       </c>
       <c r="Y22" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Z22" s="5">
         <v>10</v>
       </c>
-      <c r="AA22">
+      <c r="AA22" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="AB22" s="4">
+      <c r="AC22" s="4">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:29">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3929,12 +4039,13 @@
         <f t="shared" si="2"/>
         <v>8101</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>8131</v>
+      </c>
+      <c r="H23" t="s">
         <v>82</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
       <c r="K23">
         <v>1</v>
       </c>
@@ -3948,19 +4059,19 @@
         <v>1</v>
       </c>
       <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
         <v>20</v>
       </c>
-      <c r="P23" s="5">
-        <v>10</v>
-      </c>
       <c r="Q23" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R23" s="5">
         <v>5</v>
       </c>
       <c r="S23" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T23" s="5">
         <v>10</v>
@@ -3983,16 +4094,19 @@
       <c r="Z23" s="5">
         <v>10</v>
       </c>
-      <c r="AA23">
+      <c r="AA23" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AB23" s="4">
+      <c r="AC23" s="4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:29">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4005,22 +4119,30 @@
       <c r="F24">
         <v>8103</v>
       </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G25" si="3">G23+1</f>
+        <v>8132</v>
+      </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:29">
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F25">
         <v>8102</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>8133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G17" r:id="rId1"/>
-    <hyperlink ref="G8" r:id="rId2"/>
-    <hyperlink ref="I2" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I3" r:id="rId5"/>
+    <hyperlink ref="H17" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="J2" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId6"/>

</xml_diff>

<commit_message>
add w12 - node, python
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1260" yWindow="1440" windowWidth="31360" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Parcial 2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="138">
   <si>
     <t>Alarico Mercado Vázquez</t>
   </si>
@@ -425,6 +425,15 @@
   </si>
   <si>
     <t>Parcial 2</t>
+  </si>
+  <si>
+    <t>https://github.com/blackhawk42/administracion</t>
+  </si>
+  <si>
+    <t>node-redis</t>
+  </si>
+  <si>
+    <t>python-redis</t>
   </si>
 </sst>
 </file>
@@ -533,9 +542,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -585,7 +595,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="38">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
@@ -622,6 +632,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,8 +650,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -691,8 +702,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -743,8 +754,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -795,8 +806,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -847,8 +858,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -899,8 +910,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -951,8 +962,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1003,8 +1014,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1055,8 +1066,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1107,8 +1118,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1159,8 +1170,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1211,8 +1222,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1263,8 +1274,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1315,8 +1326,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1367,8 +1378,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1419,8 +1430,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1471,8 +1482,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1523,8 +1534,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1575,8 +1586,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1627,8 +1638,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1679,8 +1690,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1731,8 +1742,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3249,44 +3260,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="1.6640625" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
     <col min="13" max="13" width="7.1640625" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" customWidth="1"/>
-    <col min="16" max="16" width="6" style="10" customWidth="1"/>
-    <col min="17" max="17" width="6" customWidth="1"/>
-    <col min="18" max="18" width="3.83203125" customWidth="1"/>
-    <col min="19" max="19" width="3.6640625" customWidth="1"/>
-    <col min="20" max="20" width="7" customWidth="1"/>
-    <col min="21" max="21" width="4.6640625" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" customWidth="1"/>
-    <col min="23" max="23" width="4" customWidth="1"/>
-    <col min="24" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="5" customWidth="1"/>
-    <col min="26" max="26" width="3.83203125" customWidth="1"/>
-    <col min="27" max="27" width="3.6640625" style="10" customWidth="1"/>
-    <col min="28" max="28" width="10.83203125" style="4"/>
+    <col min="15" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6" style="10" customWidth="1"/>
+    <col min="19" max="19" width="6" customWidth="1"/>
+    <col min="20" max="20" width="3.83203125" customWidth="1"/>
+    <col min="21" max="21" width="3.6640625" customWidth="1"/>
+    <col min="22" max="22" width="7" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.1640625" customWidth="1"/>
+    <col min="25" max="25" width="4" customWidth="1"/>
+    <col min="26" max="26" width="10" customWidth="1"/>
+    <col min="27" max="27" width="5" customWidth="1"/>
+    <col min="28" max="28" width="3.83203125" customWidth="1"/>
+    <col min="29" max="29" width="3.6640625" style="10" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:30">
       <c r="F1" t="s">
         <v>44</v>
       </c>
@@ -3314,47 +3325,53 @@
       <c r="O1" t="s">
         <v>133</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="Q1">
-        <v>1</v>
-      </c>
-      <c r="R1">
+      <c r="S1">
+        <v>1</v>
+      </c>
+      <c r="T1">
         <v>2</v>
       </c>
-      <c r="S1">
+      <c r="U1">
         <v>3</v>
       </c>
-      <c r="T1">
+      <c r="V1">
         <v>4</v>
       </c>
-      <c r="U1">
+      <c r="W1">
         <v>5</v>
       </c>
-      <c r="V1">
+      <c r="X1">
         <v>6</v>
       </c>
-      <c r="W1">
+      <c r="Y1">
         <v>7</v>
       </c>
-      <c r="X1">
+      <c r="Z1">
         <v>8</v>
       </c>
-      <c r="Y1">
+      <c r="AA1">
         <v>9</v>
       </c>
-      <c r="Z1">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:30">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3390,24 +3407,24 @@
         <v>112</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+      <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="10">
         <v>0</v>
       </c>
       <c r="S2">
@@ -3434,16 +3451,22 @@
       <c r="Z2">
         <v>0</v>
       </c>
-      <c r="AA2" s="10">
-        <f>SUM(Q2:Z2)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4">
-        <f>AA2+P2</f>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="10">
+        <f t="shared" ref="AC2:AC23" si="0">SUM(S2:AB2)*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="4">
+        <f t="shared" ref="AD2:AD23" si="1">AC2+R2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:30">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3491,13 +3514,13 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="10">
         <v>0</v>
       </c>
       <c r="S3">
@@ -3524,16 +3547,22 @@
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AA3" s="10">
-        <f>SUM(Q3:Z3)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="4">
-        <f>AA3+P3</f>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:30">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3551,71 +3580,77 @@
         <v>51</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:H19" si="0">G3+1</f>
+        <f t="shared" ref="G4:H19" si="2">G3+1</f>
         <v>8082</v>
       </c>
       <c r="H4">
+        <f t="shared" si="2"/>
+        <v>8112</v>
+      </c>
+      <c r="I4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="10">
         <f t="shared" si="0"/>
-        <v>8112</v>
-      </c>
-      <c r="I4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="10">
-        <f>SUM(Q4:Z4)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="4">
-        <f>AA4+P4</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:30">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3635,11 +3670,11 @@
         <v>47</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8083</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8113</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -3663,13 +3698,13 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="10">
         <v>0</v>
       </c>
       <c r="S5">
@@ -3696,16 +3731,22 @@
       <c r="Z5">
         <v>0</v>
       </c>
-      <c r="AA5" s="10">
-        <f>SUM(Q5:Z5)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="4">
-        <f>AA5+P5</f>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:30">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3725,11 +3766,11 @@
         <v>52</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8084</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8114</v>
       </c>
       <c r="I6" t="s">
@@ -3753,13 +3794,13 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="10">
         <v>0</v>
       </c>
       <c r="S6">
@@ -3786,16 +3827,22 @@
       <c r="Z6">
         <v>0</v>
       </c>
-      <c r="AA6" s="10">
-        <f>SUM(Q6:Z6)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="4">
-        <f>AA6+P6</f>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:30">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3813,11 +3860,11 @@
         <v>53</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8085</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8115</v>
       </c>
       <c r="I7" t="s">
@@ -3835,13 +3882,13 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="10">
         <v>0</v>
       </c>
       <c r="S7">
@@ -3868,16 +3915,22 @@
       <c r="Z7">
         <v>0</v>
       </c>
-      <c r="AA7" s="10">
-        <f>SUM(Q7:Z7)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="4">
-        <f>AA7+P7</f>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:30">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3895,11 +3948,11 @@
         <v>54</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8086</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8116</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -3919,13 +3972,13 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="10">
         <v>0</v>
       </c>
       <c r="S8">
@@ -3952,16 +4005,22 @@
       <c r="Z8">
         <v>0</v>
       </c>
-      <c r="AA8" s="10">
-        <f>SUM(Q8:Z8)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="4">
-        <f>AA8+P8</f>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:30">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3979,11 +4038,11 @@
         <v>55</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8087</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8117</v>
       </c>
       <c r="I9" t="s">
@@ -4001,13 +4060,13 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="10">
         <v>0</v>
       </c>
       <c r="S9">
@@ -4034,16 +4093,22 @@
       <c r="Z9">
         <v>0</v>
       </c>
-      <c r="AA9" s="10">
-        <f>SUM(Q9:Z9)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="4">
-        <f>AA9+P9</f>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:30">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4061,11 +4126,11 @@
         <v>56</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8088</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8118</v>
       </c>
       <c r="I10" t="s">
@@ -4083,13 +4148,13 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="10">
         <v>0</v>
       </c>
       <c r="S10">
@@ -4116,16 +4181,22 @@
       <c r="Z10">
         <v>0</v>
       </c>
-      <c r="AA10" s="10">
-        <f>SUM(Q10:Z10)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="4">
-        <f>AA10+P10</f>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:30">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4143,11 +4214,11 @@
         <v>57</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8089</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8119</v>
       </c>
       <c r="I11" t="s">
@@ -4165,13 +4236,13 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="10">
         <v>0</v>
       </c>
       <c r="S11">
@@ -4198,16 +4269,22 @@
       <c r="Z11">
         <v>0</v>
       </c>
-      <c r="AA11" s="10">
-        <f>SUM(Q11:Z11)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="4">
-        <f>AA11+P11</f>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:30">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4225,11 +4302,11 @@
         <v>58</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8090</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8120</v>
       </c>
       <c r="I12" t="s">
@@ -4247,13 +4324,13 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="10">
+      <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="10">
         <v>0</v>
       </c>
       <c r="S12">
@@ -4280,16 +4357,22 @@
       <c r="Z12">
         <v>0</v>
       </c>
-      <c r="AA12" s="10">
-        <f>SUM(Q12:Z12)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="4">
-        <f>AA12+P12</f>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:30">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4307,11 +4390,11 @@
         <v>48</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8091</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8121</v>
       </c>
       <c r="I13" t="s">
@@ -4329,13 +4412,13 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="10">
         <v>0</v>
       </c>
       <c r="S13">
@@ -4362,16 +4445,22 @@
       <c r="Z13">
         <v>0</v>
       </c>
-      <c r="AA13" s="10">
-        <f>SUM(Q13:Z13)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="4">
-        <f>AA13+P13</f>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:30">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4389,11 +4478,11 @@
         <v>59</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8092</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8122</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -4413,13 +4502,13 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>0</v>
-      </c>
-      <c r="R14" s="5">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
         <v>0</v>
       </c>
       <c r="S14" s="5">
@@ -4446,16 +4535,22 @@
       <c r="Z14" s="5">
         <v>0</v>
       </c>
-      <c r="AA14" s="10">
-        <f>SUM(Q14:Z14)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="4">
-        <f>AA14+P14</f>
+      <c r="AA14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:30">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4473,11 +4568,11 @@
         <v>60</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8093</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8123</v>
       </c>
       <c r="I15" t="s">
@@ -4495,13 +4590,13 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15" s="10">
         <v>0</v>
       </c>
       <c r="S15" s="5">
@@ -4528,16 +4623,22 @@
       <c r="Z15" s="5">
         <v>0</v>
       </c>
-      <c r="AA15" s="10">
-        <f>SUM(Q15:Z15)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="4">
-        <f>AA15+P15</f>
+      <c r="AA15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:30">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4555,11 +4656,11 @@
         <v>61</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8094</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8124</v>
       </c>
       <c r="I16" t="s">
@@ -4577,13 +4678,13 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>0</v>
-      </c>
-      <c r="R16" s="5">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10">
         <v>0</v>
       </c>
       <c r="S16" s="5">
@@ -4610,16 +4711,22 @@
       <c r="Z16" s="5">
         <v>0</v>
       </c>
-      <c r="AA16" s="10">
-        <f>SUM(Q16:Z16)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="4">
-        <f>AA16+P16</f>
+      <c r="AA16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:30">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4637,11 +4744,11 @@
         <v>62</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8095</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8125</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -4661,13 +4768,13 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10">
         <v>0</v>
       </c>
       <c r="S17" s="5">
@@ -4694,16 +4801,22 @@
       <c r="Z17" s="5">
         <v>0</v>
       </c>
-      <c r="AA17" s="10">
-        <f>SUM(Q17:Z17)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="4">
-        <f>AA17+P17</f>
+      <c r="AA17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:30">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4721,11 +4834,11 @@
         <v>63</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8096</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8126</v>
       </c>
       <c r="I18" t="s">
@@ -4743,13 +4856,13 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="5">
-        <v>0</v>
-      </c>
-      <c r="R18" s="5">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10">
         <v>0</v>
       </c>
       <c r="S18" s="5">
@@ -4776,16 +4889,22 @@
       <c r="Z18" s="5">
         <v>0</v>
       </c>
-      <c r="AA18" s="10">
-        <f>SUM(Q18:Z18)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="4">
-        <f>AA18+P18</f>
+      <c r="AA18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:30">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4803,11 +4922,11 @@
         <v>64</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8097</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8127</v>
       </c>
       <c r="I19" t="s">
@@ -4825,13 +4944,13 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>0</v>
-      </c>
-      <c r="R19" s="5">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" s="10">
         <v>0</v>
       </c>
       <c r="S19" s="5">
@@ -4858,16 +4977,22 @@
       <c r="Z19" s="5">
         <v>0</v>
       </c>
-      <c r="AA19" s="10">
-        <f>SUM(Q19:Z19)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="4">
-        <f>AA19+P19</f>
+      <c r="AA19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:30">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4885,11 +5010,11 @@
         <v>65</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:H25" si="1">G19+1</f>
+        <f t="shared" ref="G20:H25" si="3">G19+1</f>
         <v>8098</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8128</v>
       </c>
       <c r="I20" t="s">
@@ -4907,13 +5032,13 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>0</v>
-      </c>
-      <c r="R20" s="5">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="10">
         <v>0</v>
       </c>
       <c r="S20" s="5">
@@ -4940,16 +5065,22 @@
       <c r="Z20" s="5">
         <v>0</v>
       </c>
-      <c r="AA20" s="10">
-        <f>SUM(Q20:Z20)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="4">
-        <f>AA20+P20</f>
+      <c r="AA20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:30">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4967,11 +5098,11 @@
         <v>49</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8099</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8129</v>
       </c>
       <c r="I21" t="s">
@@ -4989,13 +5120,13 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>0</v>
-      </c>
-      <c r="R21" s="5">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="10">
         <v>0</v>
       </c>
       <c r="S21" s="5">
@@ -5022,16 +5153,22 @@
       <c r="Z21" s="5">
         <v>0</v>
       </c>
-      <c r="AA21" s="10">
-        <f>SUM(Q21:Z21)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="4">
-        <f>AA21+P21</f>
+      <c r="AA21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:30">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5049,11 +5186,11 @@
         <v>50</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8100</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8130</v>
       </c>
       <c r="I22" t="s">
@@ -5071,13 +5208,13 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>0</v>
-      </c>
-      <c r="R22" s="5">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" s="10">
         <v>0</v>
       </c>
       <c r="S22" s="5">
@@ -5104,16 +5241,22 @@
       <c r="Z22" s="5">
         <v>0</v>
       </c>
-      <c r="AA22" s="10">
-        <f>SUM(Q22:Z22)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="4">
-        <f>AA22+P22</f>
+      <c r="AA22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:30">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5131,11 +5274,11 @@
         <v>66</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8101</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8131</v>
       </c>
       <c r="I23" t="s">
@@ -5153,13 +5296,13 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>0</v>
-      </c>
-      <c r="R23" s="5">
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23" s="10">
         <v>0</v>
       </c>
       <c r="S23" s="5">
@@ -5186,16 +5329,22 @@
       <c r="Z23" s="5">
         <v>0</v>
       </c>
-      <c r="AA23" s="10">
-        <f>SUM(Q23:Z23)*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="4">
-        <f>AA23+P23</f>
+      <c r="AA23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:30">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5209,11 +5358,11 @@
         <v>8103</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8132</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:30">
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
@@ -5221,7 +5370,7 @@
         <v>8102</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update excel - tareas
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="3480" yWindow="420" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Parcial 2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="149">
   <si>
     <t>Alarico Mercado Vázquez</t>
   </si>
@@ -415,12 +415,6 @@
     <t>lab questions</t>
   </si>
   <si>
-    <t>docker inegi</t>
-  </si>
-  <si>
-    <t>docker front</t>
-  </si>
-  <si>
     <t>Parcial 2</t>
   </si>
   <si>
@@ -437,6 +431,42 @@
   </si>
   <si>
     <t>https://github.com/AngelV23/AdmonIngSoft</t>
+  </si>
+  <si>
+    <t>kanban</t>
+  </si>
+  <si>
+    <t>git banching</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>front</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>front-api</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>tdd</t>
+  </si>
+  <si>
+    <t>docker maps</t>
+  </si>
+  <si>
+    <t>docker api</t>
   </si>
 </sst>
 </file>
@@ -653,8 +683,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -705,8 +735,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -757,8 +787,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -809,8 +839,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -861,8 +891,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -913,8 +943,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -965,8 +995,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1017,8 +1047,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1069,8 +1099,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1121,8 +1151,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1173,8 +1203,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1225,8 +1255,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1277,8 +1307,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1329,8 +1359,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1381,8 +1411,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1433,8 +1463,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1485,8 +1515,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1537,8 +1567,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1589,8 +1619,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1641,8 +1671,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1693,8 +1723,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1745,8 +1775,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3265,8 +3295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3275,24 +3305,25 @@
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="5" max="5" width="1.6640625" customWidth="1"/>
-    <col min="6" max="6" width="2.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="17" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
     <col min="18" max="18" width="6" style="10" customWidth="1"/>
     <col min="19" max="19" width="6" customWidth="1"/>
-    <col min="20" max="20" width="3.83203125" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
     <col min="22" max="22" width="7" customWidth="1"/>
     <col min="23" max="23" width="4.6640625" customWidth="1"/>
     <col min="24" max="24" width="10.1640625" customWidth="1"/>
-    <col min="25" max="25" width="4" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" customWidth="1"/>
     <col min="26" max="26" width="10" customWidth="1"/>
     <col min="27" max="27" width="5" customWidth="1"/>
     <col min="28" max="28" width="3.83203125" customWidth="1"/>
@@ -3320,58 +3351,58 @@
         <v>130</v>
       </c>
       <c r="M1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="N1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="O1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="S1">
-        <v>1</v>
-      </c>
-      <c r="T1">
-        <v>2</v>
-      </c>
-      <c r="U1">
-        <v>3</v>
-      </c>
-      <c r="V1">
-        <v>4</v>
-      </c>
-      <c r="W1">
-        <v>5</v>
-      </c>
-      <c r="X1">
-        <v>6</v>
-      </c>
-      <c r="Y1">
-        <v>7</v>
-      </c>
-      <c r="Z1">
-        <v>8</v>
-      </c>
-      <c r="AA1">
-        <v>9</v>
-      </c>
-      <c r="AB1">
-        <v>10</v>
+      <c r="S1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W1" t="s">
+        <v>141</v>
+      </c>
+      <c r="X1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>146</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>106</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -3591,7 +3622,7 @@
         <v>8112</v>
       </c>
       <c r="I4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -3615,42 +3646,42 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AD4" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -4052,7 +4083,7 @@
         <v>73</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -4149,7 +4180,7 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -4489,7 +4520,7 @@
         <v>8122</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -4760,7 +4791,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>1</v>

</xml_diff>